<commit_message>
finished abstract first draft. made new table
</commit_message>
<xml_diff>
--- a/ASB Data.xlsx
+++ b/ASB Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\Research\CLiMB\Projects\EMG Machine Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudius\Documents\Research\EMG Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="12012" activeTab="1" xr2:uid="{C1355271-F146-43E7-82FE-FA49F815D41B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="12015" activeTab="1" xr2:uid="{C1355271-F146-43E7-82FE-FA49F815D41B}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="86">
   <si>
     <t>Training Subject</t>
   </si>
@@ -503,13 +503,10 @@
     <t>Distal Vastus Lateralis</t>
   </si>
   <si>
-    <t>Posterior Mid Shank*</t>
+    <t>Tibialis Anterior</t>
   </si>
   <si>
-    <t>Tibialis Anterior*</t>
-  </si>
-  <si>
-    <t>Adductor Magnus**</t>
+    <t>Adductor Magnus</t>
   </si>
 </sst>
 </file>
@@ -795,28 +792,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,6 +841,24 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2262,7 +2259,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -9691,462 +9688,462 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="29"/>
-    <col min="4" max="4" width="10.109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" style="29"/>
-    <col min="10" max="12" width="11" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="29"/>
+    <col min="1" max="3" width="8.85546875" style="24"/>
+    <col min="4" max="4" width="10.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" style="24"/>
+    <col min="10" max="12" width="11" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="28" t="s">
+    <row r="5" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="E5" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="J5" s="30" t="s">
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="J5" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D6" s="31" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+    </row>
+    <row r="6" spans="4:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="D6" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="25">
         <v>2</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="25">
         <v>1</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D7" s="27" t="s">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D7" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="26">
         <v>0.94169999999999998</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="26">
         <v>0.93210000000000004</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="26">
         <v>0.96360000000000001</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="23">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="23">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="23">
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D8" s="27" t="s">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="26">
         <v>0.80630000000000002</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="26">
         <v>0.85799999999999998</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="26">
         <v>0.94120000000000004</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="23">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="23">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="23">
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="27" t="s">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D9" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="26">
         <v>0.85599999999999998</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="26">
         <v>0.88600000000000001</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="26">
         <v>0.95499999999999996</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="23">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="23">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="L9" s="27">
+      <c r="L9" s="23">
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="27" t="s">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D10" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="26">
         <v>0.92</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="26">
         <v>0.92700000000000005</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="26">
         <v>0.96799999999999997</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="23">
         <v>1E-4</v>
       </c>
-      <c r="K10" s="27">
+      <c r="K10" s="23">
         <v>1E-4</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="23">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="23" spans="4:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="31" t="s">
+    <row r="23" spans="4:8" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="D23" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="27">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D24" s="23">
         <v>0</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="26">
         <v>0</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="26">
         <v>0</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="26">
         <v>0</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="26">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="27">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D25" s="23">
         <v>1</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="26">
         <v>0.84109999999999996</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="26">
         <v>0.31819999999999998</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="26">
         <v>0.47600000000000003</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="26">
         <v>0.24600000000000002</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="27">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D26" s="23">
         <v>2</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="26">
         <v>0.91549999999999998</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="26">
         <v>0.47259999999999996</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="26">
         <v>0.58909999999999996</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="26">
         <v>0.54549999999999998</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="27">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D27" s="23">
         <v>3</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="26">
         <v>0.92949999999999999</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="26">
         <v>0.57240000000000002</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="26">
         <v>0.67359999999999998</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="26">
         <v>0.70989999999999998</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="27">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D28" s="23">
         <v>4</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="26">
         <v>0.92810000000000004</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="26">
         <v>0.64439999999999997</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="26">
         <v>0.73919999999999997</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="26">
         <v>0.79909999999999992</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="27">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D29" s="23">
         <v>5</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="26">
         <v>0.9304</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="26">
         <v>0.71109999999999995</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="26">
         <v>0.79599999999999993</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="26">
         <v>0.83319999999999994</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="27">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D30" s="23">
         <v>6</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="26">
         <v>0.93189999999999995</v>
       </c>
-      <c r="F30" s="32">
+      <c r="F30" s="26">
         <v>0.74840000000000007</v>
       </c>
-      <c r="G30" s="32">
+      <c r="G30" s="26">
         <v>0.82430000000000003</v>
       </c>
-      <c r="H30" s="32">
+      <c r="H30" s="26">
         <v>0.87620000000000009</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="27">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D31" s="23">
         <v>7</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="26">
         <v>0.9335</v>
       </c>
-      <c r="F31" s="32">
+      <c r="F31" s="26">
         <v>0.77569999999999995</v>
       </c>
-      <c r="G31" s="32">
+      <c r="G31" s="26">
         <v>0.85099999999999998</v>
       </c>
-      <c r="H31" s="32">
+      <c r="H31" s="26">
         <v>0.88939999999999997</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="27">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D32" s="23">
         <v>8</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="26">
         <v>0.93520000000000003</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="26">
         <v>0.7964</v>
       </c>
-      <c r="G32" s="32">
+      <c r="G32" s="26">
         <v>0.86280000000000001</v>
       </c>
-      <c r="H32" s="32">
+      <c r="H32" s="26">
         <v>0.90689999999999993</v>
       </c>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="27">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D33" s="23">
         <v>9</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="26">
         <v>0.93059999999999998</v>
       </c>
-      <c r="F33" s="32">
+      <c r="F33" s="26">
         <v>0.82</v>
       </c>
-      <c r="G33" s="32">
+      <c r="G33" s="26">
         <v>0.87239999999999995</v>
       </c>
-      <c r="H33" s="32">
+      <c r="H33" s="26">
         <v>0.91180000000000005</v>
       </c>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="27">
+    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D34" s="23">
         <v>10</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="26">
         <v>0.92759999999999998</v>
       </c>
-      <c r="F34" s="32">
+      <c r="F34" s="26">
         <v>0.82799999999999996</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="26">
         <v>0.87970000000000004</v>
       </c>
-      <c r="H34" s="32">
+      <c r="H34" s="26">
         <v>0.92430000000000012</v>
       </c>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="27">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D35" s="23">
         <v>11</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="26">
         <v>0.92900000000000005</v>
       </c>
-      <c r="F35" s="32">
+      <c r="F35" s="26">
         <v>0.83819999999999995</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G35" s="26">
         <v>0.88540000000000008</v>
       </c>
-      <c r="H35" s="32">
+      <c r="H35" s="26">
         <v>0.93189999999999995</v>
       </c>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="27">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D36" s="23">
         <v>12</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="26">
         <v>0.92479999999999996</v>
       </c>
-      <c r="F36" s="32">
+      <c r="F36" s="26">
         <v>0.84439999999999993</v>
       </c>
-      <c r="G36" s="32">
+      <c r="G36" s="26">
         <v>0.88980000000000004</v>
       </c>
-      <c r="H36" s="32">
+      <c r="H36" s="26">
         <v>0.94129999999999991</v>
       </c>
     </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="27">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D37" s="23">
         <v>13</v>
       </c>
-      <c r="E37" s="32">
+      <c r="E37" s="26">
         <v>0.92079999999999995</v>
       </c>
-      <c r="F37" s="32">
+      <c r="F37" s="26">
         <v>0.84909999999999997</v>
       </c>
-      <c r="G37" s="32">
+      <c r="G37" s="26">
         <v>0.89379999999999993</v>
       </c>
-      <c r="H37" s="32">
+      <c r="H37" s="26">
         <v>0.94200000000000006</v>
       </c>
     </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D38" s="27">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D38" s="23">
         <v>14</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E38" s="26">
         <v>0.92079999999999995</v>
       </c>
-      <c r="F38" s="32">
+      <c r="F38" s="26">
         <v>0.85400000000000009</v>
       </c>
-      <c r="G38" s="32">
+      <c r="G38" s="26">
         <v>0.89700000000000002</v>
       </c>
-      <c r="H38" s="32">
+      <c r="H38" s="26">
         <v>0.94739999999999991</v>
       </c>
     </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="27">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D39" s="23">
         <v>15</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E39" s="26">
         <v>0.91820000000000002</v>
       </c>
-      <c r="F39" s="32">
+      <c r="F39" s="26">
         <v>0.85970000000000002</v>
       </c>
-      <c r="G39" s="32">
+      <c r="G39" s="26">
         <v>0.9002</v>
       </c>
-      <c r="H39" s="32">
+      <c r="H39" s="26">
         <v>0.94459999999999988</v>
       </c>
     </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="27">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D40" s="23">
         <v>16</v>
       </c>
-      <c r="E40" s="32">
+      <c r="E40" s="26">
         <v>0.94650000000000001</v>
       </c>
-      <c r="F40" s="32">
+      <c r="F40" s="26">
         <v>0.86640000000000006</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G40" s="26">
         <v>0.90069999999999995</v>
       </c>
-      <c r="H40" s="32">
+      <c r="H40" s="26">
         <v>0.94010000000000005</v>
       </c>
     </row>
@@ -10162,140 +10159,265 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E1D416-0549-4E63-A5BF-B07087E90012}">
-  <dimension ref="C6:O10"/>
+  <dimension ref="C6:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="O21" sqref="O21:W24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.21875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="27" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="27" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="27" customWidth="1"/>
-    <col min="8" max="8" width="10" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="8.88671875" style="27"/>
+    <col min="3" max="3" width="10.28515625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="23" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" style="23"/>
+    <col min="15" max="15" width="9.140625" style="23" bestFit="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" customWidth="1"/>
+    <col min="21" max="21" width="19" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="35" t="s">
+    <row r="6" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="30">
         <v>1</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="31">
         <v>2</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="31">
         <v>3</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="31">
         <v>4</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="31">
         <v>5</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="31">
         <v>6</v>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="31">
         <v>7</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7" s="32">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:11" s="34" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="35" t="s">
+    <row r="8" spans="3:11" s="28" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="30">
+        <v>9</v>
+      </c>
+      <c r="E9" s="31">
+        <v>10</v>
+      </c>
+      <c r="F9" s="31">
+        <v>11</v>
+      </c>
+      <c r="G9" s="31">
+        <v>12</v>
+      </c>
+      <c r="H9" s="31">
+        <v>13</v>
+      </c>
+      <c r="I9" s="31">
+        <v>14</v>
+      </c>
+      <c r="J9" s="31">
+        <v>15</v>
+      </c>
+      <c r="K9" s="32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="H10" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="15:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="15:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O21" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="P21" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="31">
+        <v>2</v>
+      </c>
+      <c r="R21" s="31">
+        <v>3</v>
+      </c>
+      <c r="S21" s="31">
+        <v>4</v>
+      </c>
+      <c r="T21" s="31">
+        <v>5</v>
+      </c>
+      <c r="U21" s="31">
+        <v>6</v>
+      </c>
+      <c r="V21" s="31">
+        <v>7</v>
+      </c>
+      <c r="W21" s="32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="15:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O22" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="P22" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="Q22" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="R22" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="S22" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="T22" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="U22" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="V22" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="K8" s="42" t="s">
+      <c r="W22" s="36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="35" t="s">
+    <row r="23" spans="15:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O23" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="36">
+      <c r="P23" s="30">
         <v>9</v>
       </c>
-      <c r="E9" s="37">
+      <c r="Q23" s="31">
         <v>10</v>
       </c>
-      <c r="F9" s="37">
+      <c r="R23" s="31">
         <v>11</v>
       </c>
-      <c r="G9" s="37">
+      <c r="S23" s="31">
         <v>12</v>
       </c>
-      <c r="H9" s="37">
+      <c r="T23" s="31">
         <v>13</v>
       </c>
-      <c r="I9" s="37">
+      <c r="U23" s="31">
         <v>14</v>
       </c>
-      <c r="J9" s="37">
+      <c r="V23" s="31">
         <v>15</v>
       </c>
-      <c r="K9" s="38">
+      <c r="W23" s="32">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="35" t="s">
+    <row r="24" spans="15:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O24" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="P24" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="Q24" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="R24" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="44" t="s">
+      <c r="S24" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="T24" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="U24" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="V24" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="46" t="s">
+      <c r="W24" s="40" t="s">
         <v>83</v>
       </c>
     </row>
@@ -10312,32 +10434,32 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="1"/>
-    <col min="15" max="15" width="9.109375" style="1"/>
+    <col min="5" max="5" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E2" s="23" t="s">
+    <row r="2" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="I2" s="25" t="s">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="I2" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="25"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E3" s="5" t="s">
         <v>0</v>
       </c>
@@ -10348,11 +10470,11 @@
         <v>3</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E4" s="10">
         <v>1</v>
       </c>
@@ -10369,7 +10491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E5" s="10">
         <v>2</v>
       </c>
@@ -10389,7 +10511,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E6" s="10">
         <v>1</v>
       </c>
@@ -10409,7 +10531,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E7" s="10">
         <v>2</v>
       </c>
@@ -10429,7 +10551,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E8" s="10" t="s">
         <v>1</v>
       </c>
@@ -10449,7 +10571,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E9" s="10" t="s">
         <v>34</v>
       </c>
@@ -10466,7 +10588,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="I10" s="22">
         <v>8</v>
       </c>
@@ -10474,7 +10596,7 @@
         <v>0.93189999999999995</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
         <v>11</v>
       </c>
@@ -10488,7 +10610,7 @@
         <v>0.9335</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E12" s="10" t="s">
         <v>12</v>
       </c>
@@ -10499,7 +10621,7 @@
         <v>0.93520000000000003</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E13" s="10" t="s">
         <v>13</v>
       </c>
@@ -10513,7 +10635,7 @@
         <v>0.93059999999999998</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E14" s="10" t="s">
         <v>14</v>
       </c>
@@ -10527,7 +10649,7 @@
         <v>0.92759999999999998</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E15" s="10" t="s">
         <v>15</v>
       </c>
@@ -10538,7 +10660,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E16" s="10" t="s">
         <v>16</v>
       </c>
@@ -10549,7 +10671,7 @@
         <v>0.92479999999999996</v>
       </c>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E17" s="10" t="s">
         <v>17</v>
       </c>
@@ -10560,7 +10682,7 @@
         <v>0.92079999999999995</v>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I18" s="22">
         <v>6</v>
       </c>
@@ -10568,7 +10690,7 @@
         <v>0.92079999999999995</v>
       </c>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I19" s="22">
         <v>13</v>
       </c>
@@ -10576,7 +10698,7 @@
         <v>0.91820000000000002</v>
       </c>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I20" s="22">
         <v>4</v>
       </c>
@@ -10584,20 +10706,20 @@
         <v>0.94650000000000001</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="I21" s="26" t="s">
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="I21" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="26"/>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E23" s="23" t="s">
+      <c r="J21" s="45"/>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E23" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="23"/>
+      <c r="F23" s="43"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E24" s="5" t="s">
         <v>26</v>
       </c>
@@ -10608,7 +10730,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E25" s="12">
         <v>10</v>
       </c>
@@ -10616,7 +10738,7 @@
         <v>91.361099999999993</v>
       </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E26" s="12">
         <v>20</v>
       </c>
@@ -10625,7 +10747,7 @@
       </c>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="5:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E27" s="12">
         <v>30</v>
       </c>
@@ -10640,7 +10762,7 @@
       <c r="L27" s="6"/>
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E28" s="12">
         <v>40</v>
       </c>
@@ -10649,7 +10771,7 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E29" s="12">
         <v>50</v>
       </c>
@@ -10658,7 +10780,7 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E30" s="12">
         <v>60</v>
       </c>
@@ -10667,7 +10789,7 @@
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E31" s="12">
         <v>70</v>
       </c>
@@ -10676,7 +10798,7 @@
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E32" s="12">
         <v>80</v>
       </c>
@@ -10685,7 +10807,7 @@
       </c>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E33" s="12">
         <v>90</v>
       </c>
@@ -10694,7 +10816,7 @@
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E34" s="12">
         <v>100</v>
       </c>
@@ -10703,10 +10825,10 @@
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -10717,7 +10839,7 @@
       <c r="O36" s="14"/>
       <c r="P36" s="14"/>
     </row>
-    <row r="37" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -10728,7 +10850,7 @@
       <c r="O37" s="14"/>
       <c r="P37" s="14"/>
     </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -10739,7 +10861,7 @@
       <c r="O38" s="14"/>
       <c r="P38" s="14"/>
     </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -10750,7 +10872,7 @@
       <c r="O39" s="14"/>
       <c r="P39" s="14"/>
     </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -10761,7 +10883,7 @@
       <c r="O40" s="14"/>
       <c r="P40" s="14"/>
     </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -10772,7 +10894,7 @@
       <c r="O41" s="14"/>
       <c r="P41" s="14"/>
     </row>
-    <row r="42" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -10783,7 +10905,7 @@
       <c r="O42" s="14"/>
       <c r="P42" s="14"/>
     </row>
-    <row r="43" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -10794,7 +10916,7 @@
       <c r="O43" s="14"/>
       <c r="P43" s="14"/>
     </row>
-    <row r="44" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -10805,7 +10927,7 @@
       <c r="O44" s="14"/>
       <c r="P44" s="14"/>
     </row>
-    <row r="45" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -10816,7 +10938,7 @@
       <c r="O45" s="14"/>
       <c r="P45" s="14"/>
     </row>
-    <row r="46" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -10827,7 +10949,7 @@
       <c r="O46" s="14"/>
       <c r="P46" s="14"/>
     </row>
-    <row r="47" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -10838,7 +10960,7 @@
       <c r="O47" s="14"/>
       <c r="P47" s="14"/>
     </row>
-    <row r="48" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
@@ -10849,7 +10971,7 @@
       <c r="O48" s="14"/>
       <c r="P48" s="14"/>
     </row>
-    <row r="49" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
@@ -10860,7 +10982,7 @@
       <c r="O49" s="14"/>
       <c r="P49" s="14"/>
     </row>
-    <row r="50" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
@@ -10871,7 +10993,7 @@
       <c r="O50" s="14"/>
       <c r="P50" s="14"/>
     </row>
-    <row r="51" spans="8:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
@@ -10903,41 +11025,41 @@
       <selection activeCell="K5" sqref="K5:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="I2" s="25" t="s">
+    <row r="2" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E3" s="24" t="s">
+      <c r="J2" s="44"/>
+    </row>
+    <row r="3" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
@@ -10956,7 +11078,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E5" s="1">
         <v>1</v>
       </c>
@@ -10976,7 +11098,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>2</v>
       </c>
@@ -10996,7 +11118,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>1</v>
       </c>
@@ -11016,7 +11138,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>2</v>
       </c>
@@ -11036,7 +11158,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
@@ -11056,7 +11178,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="I10" s="1">
         <v>13</v>
       </c>
@@ -11064,7 +11186,7 @@
         <v>74.84</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
       <c r="G11" s="1" t="s">
         <v>41</v>
       </c>
@@ -11075,7 +11197,7 @@
         <v>77.569999999999993</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E12" s="6" t="s">
         <v>11</v>
       </c>
@@ -11089,7 +11211,7 @@
         <v>79.64</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
@@ -11100,7 +11222,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
@@ -11114,7 +11236,7 @@
         <v>82.8</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
@@ -11128,7 +11250,7 @@
         <v>83.82</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>15</v>
       </c>
@@ -11139,7 +11261,7 @@
         <v>84.44</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>16</v>
       </c>
@@ -11150,7 +11272,7 @@
         <v>84.91</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>17</v>
       </c>
@@ -11161,7 +11283,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I19" s="1">
         <v>10</v>
       </c>
@@ -11169,7 +11291,7 @@
         <v>85.97</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I20" s="1">
         <v>5</v>
       </c>
@@ -11177,51 +11299,51 @@
         <v>86.64</v>
       </c>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="I21" s="26" t="s">
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I21" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="26"/>
-    </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="J21" s="45"/>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="L25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="5:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G36" s="4"/>
     </row>
   </sheetData>
@@ -11244,39 +11366,39 @@
       <selection activeCell="K5" sqref="K5:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="I2" s="25" t="s">
+    <row r="2" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E3" s="24" t="s">
+      <c r="J2" s="44"/>
+    </row>
+    <row r="3" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-    </row>
-    <row r="4" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
@@ -11294,7 +11416,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E5" s="1">
         <v>1</v>
       </c>
@@ -11314,7 +11436,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>2</v>
       </c>
@@ -11334,7 +11456,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>1</v>
       </c>
@@ -11354,7 +11476,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>2</v>
       </c>
@@ -11374,7 +11496,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
@@ -11394,7 +11516,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="I10" s="13">
         <v>14</v>
       </c>
@@ -11402,7 +11524,7 @@
         <v>82.43</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
       <c r="I11" s="13">
         <v>15</v>
       </c>
@@ -11410,7 +11532,7 @@
         <v>85.1</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
         <v>11</v>
       </c>
@@ -11424,7 +11546,7 @@
         <v>86.28</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
@@ -11435,7 +11557,7 @@
         <v>87.24</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
@@ -11449,7 +11571,7 @@
         <v>87.97</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
@@ -11463,7 +11585,7 @@
         <v>88.54</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>15</v>
       </c>
@@ -11474,7 +11596,7 @@
         <v>88.98</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>16</v>
       </c>
@@ -11485,7 +11607,7 @@
         <v>89.38</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>17</v>
       </c>
@@ -11496,7 +11618,7 @@
         <v>89.7</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I19" s="13">
         <v>1</v>
       </c>
@@ -11504,7 +11626,7 @@
         <v>90.02</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I20" s="13">
         <v>5</v>
       </c>
@@ -11512,17 +11634,17 @@
         <v>90.07</v>
       </c>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E25" s="24" t="s">
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E25" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
       <c r="L25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="5:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E26" s="2" t="s">
         <v>7</v>
       </c>
@@ -11534,7 +11656,7 @@
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
         <v>10</v>
       </c>
@@ -11545,7 +11667,7 @@
         <v>2.2496999999999998E-6</v>
       </c>
     </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E28" s="1">
         <v>20</v>
       </c>
@@ -11556,7 +11678,7 @@
         <v>2.4534999999999999E-6</v>
       </c>
     </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29" s="1">
         <v>30</v>
       </c>
@@ -11567,7 +11689,7 @@
         <v>2.6896999999999998E-6</v>
       </c>
     </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30" s="1">
         <v>40</v>
       </c>
@@ -11578,7 +11700,7 @@
         <v>2.8829E-6</v>
       </c>
     </row>
-    <row r="31" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31" s="1">
         <v>50</v>
       </c>
@@ -11589,7 +11711,7 @@
         <v>5.9039999999999997E-6</v>
       </c>
     </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32" s="1">
         <v>60</v>
       </c>
@@ -11600,7 +11722,7 @@
         <v>6.6885999999999998E-6</v>
       </c>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" s="1">
         <v>70</v>
       </c>
@@ -11611,7 +11733,7 @@
         <v>7.2803000000000004E-6</v>
       </c>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34" s="1">
         <v>80</v>
       </c>
@@ -11642,33 +11764,33 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="5:29" x14ac:dyDescent="0.25">
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
     </row>
-    <row r="2" spans="5:29" x14ac:dyDescent="0.3">
-      <c r="I2" s="25" t="s">
+    <row r="2" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="I2" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="L2" s="25" t="s">
+      <c r="J2" s="44"/>
+      <c r="L2" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="25"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="17"/>
     </row>
-    <row r="3" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E3" s="15" t="s">
         <v>0</v>
       </c>
@@ -11679,13 +11801,13 @@
         <v>3</v>
       </c>
       <c r="H3" s="16"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="5:29" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E4" s="13">
         <v>1</v>
       </c>
@@ -11710,7 +11832,7 @@
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E5" s="13">
         <v>2</v>
       </c>
@@ -11750,7 +11872,7 @@
       <c r="AB5" s="9"/>
       <c r="AC5" s="9"/>
     </row>
-    <row r="6" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E6" s="13">
         <v>1</v>
       </c>
@@ -11775,7 +11897,7 @@
       </c>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E7" s="13">
         <v>2</v>
       </c>
@@ -11800,7 +11922,7 @@
       </c>
       <c r="N7" s="13"/>
     </row>
-    <row r="8" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E8" s="13" t="s">
         <v>1</v>
       </c>
@@ -11825,7 +11947,7 @@
       </c>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="5:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -11844,7 +11966,7 @@
       </c>
       <c r="N9" s="13"/>
     </row>
-    <row r="10" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -11863,7 +11985,7 @@
       </c>
       <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E11" s="15" t="s">
         <v>11</v>
       </c>
@@ -11886,7 +12008,7 @@
       </c>
       <c r="N11" s="13"/>
     </row>
-    <row r="12" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E12" s="13" t="s">
         <v>12</v>
       </c>
@@ -11907,7 +12029,7 @@
       </c>
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E13" s="13" t="s">
         <v>13</v>
       </c>
@@ -11930,7 +12052,7 @@
       </c>
       <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E14" s="13" t="s">
         <v>14</v>
       </c>
@@ -11953,7 +12075,7 @@
       </c>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E15" s="13" t="s">
         <v>15</v>
       </c>
@@ -11974,7 +12096,7 @@
       </c>
       <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="5:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E16" s="13" t="s">
         <v>16</v>
       </c>
@@ -11995,7 +12117,7 @@
       </c>
       <c r="N16" s="13"/>
     </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E17" s="13" t="s">
         <v>17</v>
       </c>
@@ -12016,7 +12138,7 @@
       </c>
       <c r="N17" s="13"/>
     </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -12035,7 +12157,7 @@
       </c>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
       <c r="I19" s="19">
         <v>3</v>
       </c>
@@ -12050,7 +12172,7 @@
       </c>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="I20" s="19">
         <v>11</v>
       </c>
@@ -12060,10 +12182,10 @@
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
       <c r="M21" s="13"/>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E22" s="2"/>
       <c r="I22" s="16" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
made new neural network with 100 neurons and updated results
</commit_message>
<xml_diff>
--- a/ASB Data.xlsx
+++ b/ASB Data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudius\Documents\Research\EMG Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AC4900-277A-4082-B0E7-74C677ED1899}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="12015" activeTab="1" xr2:uid="{C1355271-F146-43E7-82FE-FA49F815D41B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="12015" activeTab="3" xr2:uid="{C1355271-F146-43E7-82FE-FA49F815D41B}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="6" r:id="rId1"/>
-    <sheet name="Sensor Map" sheetId="7" r:id="rId2"/>
-    <sheet name="Random Forest" sheetId="5" r:id="rId3"/>
-    <sheet name="SVM" sheetId="4" r:id="rId4"/>
-    <sheet name="LDA" sheetId="1" r:id="rId5"/>
-    <sheet name="ANN" sheetId="3" r:id="rId6"/>
+    <sheet name="ANN" sheetId="3" r:id="rId2"/>
+    <sheet name="Sensor Map" sheetId="7" r:id="rId3"/>
+    <sheet name="Random Forest" sheetId="5" r:id="rId4"/>
+    <sheet name="SVM" sheetId="4" r:id="rId5"/>
+    <sheet name="LDA" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
   <si>
     <t>Training Subject</t>
   </si>
@@ -334,83 +335,10 @@
     <t>Normalizing features makes it worse</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">92.7 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 0.01</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">96.8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 0.01</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">90.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 0.01</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">90.3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 0.02</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">92.0 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>± 0.01</t>
-    </r>
-  </si>
-  <si>
     <t>Normalizing has negligible effect</t>
   </si>
   <si>
     <t>Normalization has no effect</t>
-  </si>
-  <si>
-    <t>Forward Selection with All Singular Values</t>
   </si>
   <si>
     <t>Classifier</t>
@@ -508,12 +436,77 @@
   <si>
     <t>Adductor Magnus</t>
   </si>
+  <si>
+    <t>Using 100 Neurons</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">94.95 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0.0077</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">95.01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0.0067</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">97.39 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0.0068</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Forward Selection with All Singular Values (10 Neurons)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -726,33 +719,33 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -768,7 +761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -777,7 +770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -786,78 +779,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -935,7 +934,7 @@
                     <c:v>3.0999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1E-4</c:v>
+                    <c:v>7.7000000000000002E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -956,7 +955,7 @@
                     <c:v>3.0999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1E-4</c:v>
+                    <c:v>7.7000000000000002E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1011,7 +1010,7 @@
                   <c:v>0.85599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92</c:v>
+                  <c:v>0.94950000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,7 +1060,7 @@
                     <c:v>5.5999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1E-4</c:v>
+                    <c:v>6.7000000000000002E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1082,7 +1081,7 @@
                     <c:v>5.5999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1E-4</c:v>
+                    <c:v>6.7000000000000002E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1137,7 +1136,7 @@
                   <c:v>0.88600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92700000000000005</c:v>
+                  <c:v>0.95009999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1186,7 +1185,7 @@
                     <c:v>2.8E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1E-4</c:v>
+                    <c:v>8.6E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1207,7 +1206,7 @@
                     <c:v>2.8E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1E-4</c:v>
+                    <c:v>8.6E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1262,7 +1261,7 @@
                   <c:v>0.95499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96799999999999997</c:v>
+                  <c:v>0.97389999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2118,52 +2117,52 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24600000000000002</c:v>
+                  <c:v>0.27150000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54549999999999998</c:v>
+                  <c:v>0.57030000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70989999999999998</c:v>
+                  <c:v>0.72850000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79909999999999992</c:v>
+                  <c:v>0.8286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83319999999999994</c:v>
+                  <c:v>0.872</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87620000000000009</c:v>
+                  <c:v>0.90500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.88939999999999997</c:v>
+                  <c:v>0.92479999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90689999999999993</c:v>
+                  <c:v>0.94810000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.91180000000000005</c:v>
+                  <c:v>0.94499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.92430000000000012</c:v>
+                  <c:v>0.95069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.93189999999999995</c:v>
+                  <c:v>0.95540000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.94129999999999991</c:v>
+                  <c:v>0.95830000000000004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.94200000000000006</c:v>
+                  <c:v>0.96079999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.94739999999999991</c:v>
+                  <c:v>0.96220000000000006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.94459999999999988</c:v>
+                  <c:v>0.96630000000000005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.94010000000000005</c:v>
+                  <c:v>0.96650000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2287,6 +2286,7 @@
         <c:axId val="553206224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2489,6 +2489,434 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ANN!$J$5:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>27.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.849999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.86</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95.07</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>95.83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96.08</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>96.22</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96.63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-093E-4576-9605-8A4BF05E5B54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ANN!$M$5:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>27.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.239999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89.29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>93.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93.92</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>93.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-093E-4576-9605-8A4BF05E5B54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="507280168"/>
+        <c:axId val="507281808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="507280168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507281808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="507281808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507280168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2853,7 +3281,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3180,7 +3608,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3542,7 +3970,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3908,7 +4336,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4191,434 +4619,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>ANN!$J$5:$J$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>24.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.55</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70.989999999999995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>79.91</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>83.32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87.62</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>88.94</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90.69</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>91.18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>92.43</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>93.19</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>94.13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>94.74</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>94.46</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-093E-4576-9605-8A4BF05E5B54}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>ANN!$M$5:$M$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>27.47</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>55.38</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>72.08</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80.239999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>83.11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>85.94</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>88.91</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>89.29</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90.23</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>91.11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>93.52</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>92.9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>93.68</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>93.92</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>93.61</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-093E-4576-9605-8A4BF05E5B54}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="507280168"/>
-        <c:axId val="507281808"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="507280168"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="507281808"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="507281808"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="507280168"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5990,7 +5990,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6017,8 +6017,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6119,7 +6119,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6151,10 +6151,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6194,23 +6194,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6315,8 +6314,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6448,20 +6447,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6475,17 +6473,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -8570,7 +8557,7 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8597,8 +8584,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8699,7 +8686,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -8731,10 +8718,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -8774,22 +8761,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -8894,8 +8882,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9027,19 +9015,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -9053,6 +9042,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9153,6 +9153,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8DB8730-6FDD-496A-BE27-BD0881C418EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>36</xdr:row>
@@ -9190,7 +9231,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9231,7 +9272,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9336,47 +9377,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8DB8730-6FDD-496A-BE27-BD0881C418EA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9684,8 +9684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10261E67-292F-46B7-B437-2C91A5769C1C}">
   <dimension ref="D5:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9700,20 +9700,20 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="J5" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="J5" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
     </row>
     <row r="6" spans="4:12" ht="15" x14ac:dyDescent="0.2">
       <c r="D6" s="25" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>1</v>
@@ -9725,7 +9725,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J6" s="25" t="s">
         <v>1</v>
@@ -9739,7 +9739,7 @@
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D7" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" s="26">
         <v>0.94169999999999998</v>
@@ -9751,7 +9751,7 @@
         <v>0.96360000000000001</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J7" s="23">
         <v>3.2000000000000002E-3</v>
@@ -9765,7 +9765,7 @@
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D8" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E8" s="26">
         <v>0.80630000000000002</v>
@@ -9777,7 +9777,7 @@
         <v>0.94120000000000004</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J8" s="23">
         <v>1.0999999999999999E-2</v>
@@ -9791,7 +9791,7 @@
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D9" s="23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E9" s="26">
         <v>0.85599999999999998</v>
@@ -9803,7 +9803,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J9" s="23">
         <v>3.0999999999999999E-3</v>
@@ -9817,45 +9817,45 @@
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D10" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E10" s="26">
-        <v>0.92</v>
+        <v>0.94950000000000001</v>
       </c>
       <c r="F10" s="26">
-        <v>0.92700000000000005</v>
+        <v>0.95009999999999994</v>
       </c>
       <c r="G10" s="26">
-        <v>0.96799999999999997</v>
+        <v>0.97389999999999999</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="J10" s="23">
-        <v>1E-4</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="K10" s="23">
-        <v>1E-4</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="L10" s="23">
-        <v>1E-4</v>
+        <v>8.6E-3</v>
       </c>
     </row>
     <row r="23" spans="4:8" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D23" s="25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.2">
@@ -9889,7 +9889,7 @@
         <v>0.47600000000000003</v>
       </c>
       <c r="H25" s="26">
-        <v>0.24600000000000002</v>
+        <v>0.27150000000000002</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.2">
@@ -9906,7 +9906,7 @@
         <v>0.58909999999999996</v>
       </c>
       <c r="H26" s="26">
-        <v>0.54549999999999998</v>
+        <v>0.57030000000000003</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.2">
@@ -9923,7 +9923,7 @@
         <v>0.67359999999999998</v>
       </c>
       <c r="H27" s="26">
-        <v>0.70989999999999998</v>
+        <v>0.72850000000000004</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.2">
@@ -9940,7 +9940,7 @@
         <v>0.73919999999999997</v>
       </c>
       <c r="H28" s="26">
-        <v>0.79909999999999992</v>
+        <v>0.8286</v>
       </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.2">
@@ -9957,7 +9957,7 @@
         <v>0.79599999999999993</v>
       </c>
       <c r="H29" s="26">
-        <v>0.83319999999999994</v>
+        <v>0.872</v>
       </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.2">
@@ -9974,7 +9974,7 @@
         <v>0.82430000000000003</v>
       </c>
       <c r="H30" s="26">
-        <v>0.87620000000000009</v>
+        <v>0.90500000000000003</v>
       </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.2">
@@ -9991,7 +9991,7 @@
         <v>0.85099999999999998</v>
       </c>
       <c r="H31" s="26">
-        <v>0.88939999999999997</v>
+        <v>0.92479999999999996</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.2">
@@ -10008,7 +10008,7 @@
         <v>0.86280000000000001</v>
       </c>
       <c r="H32" s="26">
-        <v>0.90689999999999993</v>
+        <v>0.94810000000000005</v>
       </c>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.2">
@@ -10025,7 +10025,7 @@
         <v>0.87239999999999995</v>
       </c>
       <c r="H33" s="26">
-        <v>0.91180000000000005</v>
+        <v>0.94499999999999995</v>
       </c>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.2">
@@ -10042,7 +10042,7 @@
         <v>0.87970000000000004</v>
       </c>
       <c r="H34" s="26">
-        <v>0.92430000000000012</v>
+        <v>0.95069999999999999</v>
       </c>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.2">
@@ -10059,7 +10059,7 @@
         <v>0.88540000000000008</v>
       </c>
       <c r="H35" s="26">
-        <v>0.93189999999999995</v>
+        <v>0.95540000000000003</v>
       </c>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.2">
@@ -10076,7 +10076,7 @@
         <v>0.88980000000000004</v>
       </c>
       <c r="H36" s="26">
-        <v>0.94129999999999991</v>
+        <v>0.95830000000000004</v>
       </c>
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.2">
@@ -10093,7 +10093,7 @@
         <v>0.89379999999999993</v>
       </c>
       <c r="H37" s="26">
-        <v>0.94200000000000006</v>
+        <v>0.96079999999999999</v>
       </c>
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.2">
@@ -10110,7 +10110,7 @@
         <v>0.89700000000000002</v>
       </c>
       <c r="H38" s="26">
-        <v>0.94739999999999991</v>
+        <v>0.96220000000000006</v>
       </c>
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.2">
@@ -10127,7 +10127,7 @@
         <v>0.9002</v>
       </c>
       <c r="H39" s="26">
-        <v>0.94459999999999988</v>
+        <v>0.96630000000000005</v>
       </c>
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.2">
@@ -10144,7 +10144,7 @@
         <v>0.90069999999999995</v>
       </c>
       <c r="H40" s="26">
-        <v>0.94010000000000005</v>
+        <v>0.96650000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -10158,10 +10158,482 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB1CB2D-1AAF-4F21-A838-686EEC42B733}">
+  <dimension ref="E1:AC41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+    </row>
+    <row r="2" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="I2" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="46"/>
+      <c r="L2" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" s="46"/>
+      <c r="N2" s="17"/>
+    </row>
+    <row r="3" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="5:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="13"/>
+    </row>
+    <row r="5" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E5" s="13">
+        <v>2</v>
+      </c>
+      <c r="F5" s="13">
+        <v>2</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="19">
+        <v>12</v>
+      </c>
+      <c r="J5" s="19">
+        <v>27.15</v>
+      </c>
+      <c r="L5" s="19">
+        <v>12</v>
+      </c>
+      <c r="M5" s="19">
+        <v>27.47</v>
+      </c>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+    </row>
+    <row r="6" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="19">
+        <v>13</v>
+      </c>
+      <c r="J6" s="19">
+        <v>57.03</v>
+      </c>
+      <c r="L6" s="19">
+        <v>3</v>
+      </c>
+      <c r="M6" s="19">
+        <v>55.38</v>
+      </c>
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E7" s="13">
+        <v>2</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="19">
+        <v>8</v>
+      </c>
+      <c r="J7" s="19">
+        <v>72.849999999999994</v>
+      </c>
+      <c r="L7" s="19">
+        <v>7</v>
+      </c>
+      <c r="M7" s="19">
+        <v>72.08</v>
+      </c>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="19">
+        <v>1</v>
+      </c>
+      <c r="J8" s="19">
+        <v>82.86</v>
+      </c>
+      <c r="L8" s="19">
+        <v>5</v>
+      </c>
+      <c r="M8" s="19">
+        <v>80.239999999999995</v>
+      </c>
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="5:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="19">
+        <v>7</v>
+      </c>
+      <c r="J9" s="19">
+        <v>87.2</v>
+      </c>
+      <c r="L9" s="19">
+        <v>14</v>
+      </c>
+      <c r="M9" s="19">
+        <v>83.11</v>
+      </c>
+      <c r="N9" s="13"/>
+    </row>
+    <row r="10" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="19">
+        <v>10</v>
+      </c>
+      <c r="J10" s="19">
+        <v>90.5</v>
+      </c>
+      <c r="L10" s="19">
+        <v>4</v>
+      </c>
+      <c r="M10" s="19">
+        <v>85.94</v>
+      </c>
+      <c r="N10" s="13"/>
+    </row>
+    <row r="11" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="19">
+        <v>3</v>
+      </c>
+      <c r="J11" s="19">
+        <v>92.48</v>
+      </c>
+      <c r="L11" s="19">
+        <v>9</v>
+      </c>
+      <c r="M11" s="19">
+        <v>88.91</v>
+      </c>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="19">
+        <v>15</v>
+      </c>
+      <c r="J12" s="19">
+        <v>94.81</v>
+      </c>
+      <c r="L12" s="19">
+        <v>10</v>
+      </c>
+      <c r="M12" s="19">
+        <v>89.29</v>
+      </c>
+      <c r="N12" s="13"/>
+    </row>
+    <row r="13" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="19">
+        <v>4</v>
+      </c>
+      <c r="J13" s="19">
+        <v>94.5</v>
+      </c>
+      <c r="L13" s="19">
+        <v>15</v>
+      </c>
+      <c r="M13" s="19">
+        <v>90.23</v>
+      </c>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="19">
+        <v>6</v>
+      </c>
+      <c r="J14" s="19">
+        <v>95.07</v>
+      </c>
+      <c r="L14" s="19">
+        <v>6</v>
+      </c>
+      <c r="M14" s="19">
+        <v>91.11</v>
+      </c>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="19">
+        <v>16</v>
+      </c>
+      <c r="J15" s="19">
+        <v>95.54</v>
+      </c>
+      <c r="L15" s="19">
+        <v>13</v>
+      </c>
+      <c r="M15" s="19">
+        <v>93.52</v>
+      </c>
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="19">
+        <v>5</v>
+      </c>
+      <c r="J16" s="19">
+        <v>95.83</v>
+      </c>
+      <c r="L16" s="19">
+        <v>16</v>
+      </c>
+      <c r="M16" s="19">
+        <v>92.9</v>
+      </c>
+      <c r="N16" s="13"/>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="19">
+        <v>9</v>
+      </c>
+      <c r="J17" s="19">
+        <v>96.08</v>
+      </c>
+      <c r="L17" s="19">
+        <v>2</v>
+      </c>
+      <c r="M17" s="19">
+        <v>93.68</v>
+      </c>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="19">
+        <v>2</v>
+      </c>
+      <c r="J18" s="19">
+        <v>96.22</v>
+      </c>
+      <c r="L18" s="19">
+        <v>8</v>
+      </c>
+      <c r="M18" s="19">
+        <v>93.92</v>
+      </c>
+      <c r="N18" s="13"/>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I19" s="19">
+        <v>11</v>
+      </c>
+      <c r="J19" s="19">
+        <v>96.63</v>
+      </c>
+      <c r="L19" s="19">
+        <v>11</v>
+      </c>
+      <c r="M19" s="19">
+        <v>93.61</v>
+      </c>
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I20" s="19">
+        <v>14</v>
+      </c>
+      <c r="J20" s="19">
+        <v>96.71</v>
+      </c>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="I22" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="M22" s="13"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="48"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="42"/>
+      <c r="G36" s="42"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="41"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="41"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="41"/>
+      <c r="G39" s="41"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="41"/>
+      <c r="G40" s="41"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="41"/>
+      <c r="G41" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="E35:F35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E1D416-0549-4E63-A5BF-B07087E90012}">
   <dimension ref="C6:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21:W24"/>
     </sheetView>
   </sheetViews>
@@ -10219,31 +10691,31 @@
     </row>
     <row r="8" spans="3:11" s="28" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="29" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10277,31 +10749,31 @@
     </row>
     <row r="10" spans="3:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>78</v>
-      </c>
       <c r="E10" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>85</v>
-      </c>
       <c r="H10" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I10" s="38" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K10" s="40" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="15:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -10336,31 +10808,31 @@
     </row>
     <row r="22" spans="15:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O22" s="29" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="P22" s="33" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q22" s="34" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="R22" s="35" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="S22" s="35" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="T22" s="35" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="U22" s="35" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="V22" s="35" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="W22" s="36" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="15:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10394,31 +10866,31 @@
     </row>
     <row r="24" spans="15:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O24" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="P24" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="P24" s="37" t="s">
-        <v>78</v>
-      </c>
       <c r="Q24" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="R24" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="S24" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="R24" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="S24" s="39" t="s">
-        <v>85</v>
-      </c>
       <c r="T24" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="U24" s="38" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="V24" s="39" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="W24" s="40" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -10426,12 +10898,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94775D0D-450F-4CB0-98B6-7835CCF1C2F2}">
   <dimension ref="E2:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10448,15 +10920,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="I2" s="44" t="s">
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="I2" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="44"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="9"/>
     </row>
     <row r="3" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10470,8 +10942,8 @@
         <v>3</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="5:11" x14ac:dyDescent="0.25">
@@ -10508,7 +10980,7 @@
         <v>0.84109999999999996</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="5:11" x14ac:dyDescent="0.25">
@@ -10528,7 +11000,7 @@
         <v>0.91549999999999998</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="5:11" x14ac:dyDescent="0.25">
@@ -10548,7 +11020,7 @@
         <v>0.92949999999999999</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="5:11" x14ac:dyDescent="0.25">
@@ -10568,7 +11040,7 @@
         <v>0.92810000000000004</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="5:11" x14ac:dyDescent="0.25">
@@ -10585,7 +11057,7 @@
         <v>0.9304</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="5:11" x14ac:dyDescent="0.25">
@@ -10707,16 +11179,16 @@
       </c>
     </row>
     <row r="21" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="I21" s="45" t="s">
+      <c r="I21" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="45"/>
+      <c r="J21" s="47"/>
     </row>
     <row r="23" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="43"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
@@ -10727,7 +11199,7 @@
         <v>27</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="5:15" x14ac:dyDescent="0.25">
@@ -11017,7 +11489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060203B5-DCCC-4096-B09B-C493C4DA26F8}">
   <dimension ref="E1:L36"/>
   <sheetViews>
@@ -11044,19 +11516,19 @@
       <c r="J1" s="13"/>
     </row>
     <row r="2" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="44"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="16"/>
     </row>
     <row r="4" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11095,7 +11567,7 @@
         <v>31.82</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="5:11" x14ac:dyDescent="0.25">
@@ -11115,7 +11587,7 @@
         <v>47.26</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="5:11" x14ac:dyDescent="0.25">
@@ -11135,7 +11607,7 @@
         <v>57.24</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="5:11" x14ac:dyDescent="0.25">
@@ -11155,7 +11627,7 @@
         <v>64.44</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="5:11" x14ac:dyDescent="0.25">
@@ -11175,7 +11647,7 @@
         <v>71.11</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="5:11" x14ac:dyDescent="0.25">
@@ -11300,10 +11772,10 @@
       </c>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="I21" s="45" t="s">
+      <c r="I21" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="45"/>
+      <c r="J21" s="47"/>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="L25" t="s">
@@ -11358,7 +11830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EDACF1-6682-4AB2-A0FD-FFC4F2C29D9C}">
   <dimension ref="E1:L34"/>
   <sheetViews>
@@ -11384,19 +11856,19 @@
       <c r="J1" s="13"/>
     </row>
     <row r="2" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="44"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
     </row>
     <row r="4" spans="5:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
@@ -11433,7 +11905,7 @@
         <v>47.6</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="5:11" x14ac:dyDescent="0.25">
@@ -11453,7 +11925,7 @@
         <v>58.91</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="5:11" x14ac:dyDescent="0.25">
@@ -11473,7 +11945,7 @@
         <v>67.36</v>
       </c>
       <c r="K7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="5:11" x14ac:dyDescent="0.25">
@@ -11493,7 +11965,7 @@
         <v>73.92</v>
       </c>
       <c r="K8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="5:11" x14ac:dyDescent="0.25">
@@ -11513,7 +11985,7 @@
         <v>79.599999999999994</v>
       </c>
       <c r="K9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="5:11" x14ac:dyDescent="0.25">
@@ -11635,11 +12107,11 @@
       </c>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
       <c r="L25" t="s">
         <v>44</v>
       </c>
@@ -11754,451 +12226,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB1CB2D-1AAF-4F21-A838-686EEC42B733}">
-  <dimension ref="E1:AC22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-    </row>
-    <row r="2" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="I2" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="44"/>
-      <c r="L2" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="17"/>
-    </row>
-    <row r="3" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="5:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="13">
-        <v>1</v>
-      </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E5" s="13">
-        <v>2</v>
-      </c>
-      <c r="F5" s="13">
-        <v>2</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="19">
-        <v>2</v>
-      </c>
-      <c r="J5" s="19">
-        <v>24.6</v>
-      </c>
-      <c r="L5" s="19">
-        <v>12</v>
-      </c>
-      <c r="M5" s="19">
-        <v>27.47</v>
-      </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-    </row>
-    <row r="6" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E6" s="13">
-        <v>1</v>
-      </c>
-      <c r="F6" s="13">
-        <v>2</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="19">
-        <v>13</v>
-      </c>
-      <c r="J6" s="19">
-        <v>54.55</v>
-      </c>
-      <c r="L6" s="19">
-        <v>3</v>
-      </c>
-      <c r="M6" s="19">
-        <v>55.38</v>
-      </c>
-      <c r="N6" s="13"/>
-    </row>
-    <row r="7" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E7" s="13">
-        <v>2</v>
-      </c>
-      <c r="F7" s="13">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="19">
-        <v>12</v>
-      </c>
-      <c r="J7" s="19">
-        <v>70.989999999999995</v>
-      </c>
-      <c r="L7" s="19">
-        <v>7</v>
-      </c>
-      <c r="M7" s="19">
-        <v>72.08</v>
-      </c>
-      <c r="N7" s="13"/>
-    </row>
-    <row r="8" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="19">
-        <v>10</v>
-      </c>
-      <c r="J8" s="19">
-        <v>79.91</v>
-      </c>
-      <c r="L8" s="19">
-        <v>5</v>
-      </c>
-      <c r="M8" s="19">
-        <v>80.239999999999995</v>
-      </c>
-      <c r="N8" s="13"/>
-    </row>
-    <row r="9" spans="5:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="19">
-        <v>9</v>
-      </c>
-      <c r="J9" s="19">
-        <v>83.32</v>
-      </c>
-      <c r="L9" s="19">
-        <v>14</v>
-      </c>
-      <c r="M9" s="19">
-        <v>83.11</v>
-      </c>
-      <c r="N9" s="13"/>
-    </row>
-    <row r="10" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="19">
-        <v>4</v>
-      </c>
-      <c r="J10" s="19">
-        <v>87.62</v>
-      </c>
-      <c r="L10" s="19">
-        <v>4</v>
-      </c>
-      <c r="M10" s="19">
-        <v>85.94</v>
-      </c>
-      <c r="N10" s="13"/>
-    </row>
-    <row r="11" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="19">
-        <v>7</v>
-      </c>
-      <c r="J11" s="19">
-        <v>88.94</v>
-      </c>
-      <c r="L11" s="19">
-        <v>9</v>
-      </c>
-      <c r="M11" s="19">
-        <v>88.91</v>
-      </c>
-      <c r="N11" s="13"/>
-    </row>
-    <row r="12" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="19">
-        <v>8</v>
-      </c>
-      <c r="J12" s="19">
-        <v>90.69</v>
-      </c>
-      <c r="L12" s="19">
-        <v>10</v>
-      </c>
-      <c r="M12" s="19">
-        <v>89.29</v>
-      </c>
-      <c r="N12" s="13"/>
-    </row>
-    <row r="13" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="19">
-        <v>5</v>
-      </c>
-      <c r="J13" s="19">
-        <v>91.18</v>
-      </c>
-      <c r="L13" s="19">
-        <v>15</v>
-      </c>
-      <c r="M13" s="19">
-        <v>90.23</v>
-      </c>
-      <c r="N13" s="13"/>
-    </row>
-    <row r="14" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="19">
-        <v>6</v>
-      </c>
-      <c r="J14" s="19">
-        <v>92.43</v>
-      </c>
-      <c r="L14" s="19">
-        <v>6</v>
-      </c>
-      <c r="M14" s="19">
-        <v>91.11</v>
-      </c>
-      <c r="N14" s="13"/>
-    </row>
-    <row r="15" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E15" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="19">
-        <v>16</v>
-      </c>
-      <c r="J15" s="19">
-        <v>93.19</v>
-      </c>
-      <c r="L15" s="19">
-        <v>13</v>
-      </c>
-      <c r="M15" s="19">
-        <v>93.52</v>
-      </c>
-      <c r="N15" s="13"/>
-    </row>
-    <row r="16" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="19">
-        <v>1</v>
-      </c>
-      <c r="J16" s="19">
-        <v>94.13</v>
-      </c>
-      <c r="L16" s="19">
-        <v>16</v>
-      </c>
-      <c r="M16" s="19">
-        <v>92.9</v>
-      </c>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E17" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="19">
-        <v>15</v>
-      </c>
-      <c r="J17" s="19">
-        <v>94.2</v>
-      </c>
-      <c r="L17" s="19">
-        <v>2</v>
-      </c>
-      <c r="M17" s="19">
-        <v>93.68</v>
-      </c>
-      <c r="N17" s="13"/>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="19">
-        <v>14</v>
-      </c>
-      <c r="J18" s="19">
-        <v>94.74</v>
-      </c>
-      <c r="L18" s="19">
-        <v>8</v>
-      </c>
-      <c r="M18" s="19">
-        <v>93.92</v>
-      </c>
-      <c r="N18" s="13"/>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I19" s="19">
-        <v>3</v>
-      </c>
-      <c r="J19" s="19">
-        <v>94.46</v>
-      </c>
-      <c r="L19" s="19">
-        <v>11</v>
-      </c>
-      <c r="M19" s="19">
-        <v>93.61</v>
-      </c>
-      <c r="N19" s="13"/>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I20" s="19">
-        <v>11</v>
-      </c>
-      <c r="J20" s="19">
-        <v>94.01</v>
-      </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="M21" s="13"/>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E22" s="2"/>
-      <c r="I22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M22" s="13"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="L2:M3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>